<commit_message>
avances admin, falta cambiar logins y crear agentes y organizaciones desde admin
</commit_message>
<xml_diff>
--- a/Codigo/src/main/resources/uploads/'2'.xlsx
+++ b/Codigo/src/main/resources/uploads/'2'.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultad\3er año 2022\Diseño de sistemas\2022-ma-ma-mama-grupo-05\Codigo\excelsDePrueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48531200-8CBB-4B34-BF9B-8AA465292616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFC6A88F-6F24-4DA7-AA34-B966DB385503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="3765" windowWidth="17280" windowHeight="8970" xr2:uid="{EC2C0D61-4338-4D5B-A2AC-721C13D9CD63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ADC403D9-879F-4B3F-99C0-F9611F8E680D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>Actividad</t>
   </si>
@@ -42,9 +42,6 @@
     <t>COMBUSTION_FIJA</t>
   </si>
   <si>
-    <t>GAS_NATURAL</t>
-  </si>
-  <si>
     <t>MENSUAL</t>
   </si>
   <si>
@@ -67,6 +64,24 @@
   </si>
   <si>
     <t>PESO</t>
+  </si>
+  <si>
+    <t>DIESEL</t>
+  </si>
+  <si>
+    <t>KEROSENE</t>
+  </si>
+  <si>
+    <t>FUEL_OIL</t>
+  </si>
+  <si>
+    <t>NAFTA</t>
+  </si>
+  <si>
+    <t>CARBON_DE_LEÑA</t>
+  </si>
+  <si>
+    <t>LEÑA</t>
   </si>
 </sst>
 </file>
@@ -418,14 +433,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACCF765-8B55-414D-AE75-F778505838C5}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{481884F5-EDAE-4D53-AB3E-903165C744C2}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -449,84 +471,169 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>44652</v>
+        <v>44856</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>44682</v>
+        <v>44887</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>44682</v>
+        <v>44887</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>44682</v>
+        <v>44887</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>800</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>44682</v>
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44856</v>
       </c>
     </row>
   </sheetData>

</xml_diff>